<commit_message>
Builder and cases adapted with battery block
</commit_message>
<xml_diff>
--- a/main/Cases/Example3.xlsx
+++ b/main/Cases/Example3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergi Costa\Documents\agistin\main\Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb8ea44fc11ff6bc/Documentos/Universitat/CITCEA/agistin/main/Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F10576-D163-4FFA-8A81-72574DDBB5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{55806C53-CE58-44BE-9F56-1478E0E56E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04A31A57-BBE1-415B-92A8-3EBFA616FC03}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" firstSheet="2" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Grid" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="NewPump" sheetId="7" r:id="rId10"/>
     <sheet name="Turbine" sheetId="8" r:id="rId11"/>
     <sheet name="Switch" sheetId="11" r:id="rId12"/>
+    <sheet name="Battery_Ex0" sheetId="13" r:id="rId13"/>
+    <sheet name="Battery" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -135,6 +137,39 @@
   </si>
   <si>
     <t>PV</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>Emax</t>
+  </si>
+  <si>
+    <t>Emin</t>
+  </si>
+  <si>
+    <t>SOCmax</t>
+  </si>
+  <si>
+    <t>SOCmin</t>
+  </si>
+  <si>
+    <t>Einst</t>
+  </si>
+  <si>
+    <t>rend_ch</t>
+  </si>
+  <si>
+    <t>rend_disc</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -170,9 +205,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,7 +227,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -489,16 +525,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDBFD1F-93C1-4DFD-8CBE-DA36DEB8F281}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,12 +545,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="1">
-        <v>100000</v>
+        <v>480000</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -533,12 +569,12 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,12 +598,12 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,8 +625,161 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15FA2B1-0AD0-433C-A487-578A0168C448}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="12.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>100000</v>
+      </c>
+      <c r="H2">
+        <v>80000</v>
+      </c>
+      <c r="I2">
+        <v>80000</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D4C620-E061-4F0D-A37B-4B2D6EF3E2AE}">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="12.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -600,15 +789,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,12 +814,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -639,18 +828,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -663,15 +852,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -714,16 +903,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FF505B-0D98-41A1-A611-0C6A30A0D663}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="9" max="9" width="23.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -782,7 +971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -825,12 +1014,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -838,7 +1027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -859,17 +1048,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -883,16 +1072,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB1DA86-E473-4447-9EDD-C35A3EE02889}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +1095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -933,12 +1122,12 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -974,12 +1163,12 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update 01.07.2024 SCO is working
</commit_message>
<xml_diff>
--- a/main/Cases/Example3.xlsx
+++ b/main/Cases/Example3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb8ea44fc11ff6bc/Documentos/Universitat/CITCEA/agistin/main/Cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvalois\Desktop\Current Projects\AGISTIN\GitHub Repositories\Uni-Kassel_Task-3.2\agistin\main\Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{55806C53-CE58-44BE-9F56-1478E0E56E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04A31A57-BBE1-415B-92A8-3EBFA616FC03}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6A722B-4435-4922-88A8-46D24B09C642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" firstSheet="2" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
+    <workbookView xWindow="-38520" yWindow="-3315" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Grid" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -205,13 +205,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -227,9 +226,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,7 +266,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -373,7 +372,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,16 +524,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDBFD1F-93C1-4DFD-8CBE-DA36DEB8F281}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -569,12 +568,12 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -598,12 +597,12 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +624,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -633,18 +632,18 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15FA2B1-0AD0-433C-A487-578A0168C448}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="10" max="10" width="12.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -682,11 +681,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>100</v>
       </c>
       <c r="C2">
@@ -719,9 +718,6 @@
       <c r="L2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -736,12 +732,12 @@
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="10" max="10" width="12.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -792,12 +788,12 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="5" max="5" width="22.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -814,7 +810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -828,7 +824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -855,12 +851,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -877,7 +873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -907,12 +903,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="9" max="9" width="23.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -941,7 +937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -971,7 +967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1014,12 +1010,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1048,17 +1044,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1070,18 +1066,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB1DA86-E473-4447-9EDD-C35A3EE02889}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1089,13 +1085,16 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1103,9 +1102,12 @@
         <v>50000</v>
       </c>
       <c r="C2" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D2" s="1">
         <v>100000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1122,12 +1124,12 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="7" max="7" width="22.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1163,12 +1165,12 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update 12.08.2024 Sumulation results showing different results
</commit_message>
<xml_diff>
--- a/main/Cases/Example3.xlsx
+++ b/main/Cases/Example3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvalois\Desktop\Current Projects\AGISTIN\GitHub Repositories\Uni-Kassel_Task-3.2\agistin\main\Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvalois\Desktop\CurrentProjects\AGISTIN\GitHub Repositories\Uni-Kassel_Task-3.2\agistin\main\Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6A722B-4435-4922-88A8-46D24B09C642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1ECE6B-7522-42F8-95DF-AB12A3B4E922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3315" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Grid" sheetId="1" r:id="rId1"/>
@@ -1069,7 +1069,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>